<commit_message>
- FIX: Added missing row/column columns to trait data templates.
</commit_message>
<xml_diff>
--- a/trials-data/example-trials-data.xlsx
+++ b/trials-data/example-trials-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\trials-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5450D762-9865-4FEE-A041-6EF7F7274392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB542CF-022F-409C-91BD-E986D2B6A4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="3" r:id="rId1"/>
@@ -2264,7 +2264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2722,7 +2722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- ADD: Added set size and timeseries flag to trials template.
</commit_message>
<xml_diff>
--- a/trials-data/example-trials-data.xlsx
+++ b/trials-data/example-trials-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\trials-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6A2105-1409-47FF-8B67-C930E4948BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0630D4AB-4109-46DB-964D-A3879C2A613C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="38700" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3696" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3698" uniqueCount="459">
   <si>
     <t>Name</t>
   </si>
@@ -1421,6 +1421,12 @@
   </si>
   <si>
     <t>[["Spring", "Winter"]]</t>
+  </si>
+  <si>
+    <t>Set size</t>
+  </si>
+  <si>
+    <t>Is timeseries</t>
   </si>
 </sst>
 </file>
@@ -1863,9 +1869,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDF6150C-EB7C-4511-B47B-2F8122570053}" name="Table136" displayName="Table136" ref="A1:J7" totalsRowShown="0">
-  <autoFilter ref="A1:J7" xr:uid="{4E670C69-5459-4D42-BBD4-1C0FE57A115B}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDF6150C-EB7C-4511-B47B-2F8122570053}" name="Table136" displayName="Table136" ref="A1:L7" totalsRowShown="0">
+  <autoFilter ref="A1:L7" xr:uid="{4E670C69-5459-4D42-BBD4-1C0FE57A115B}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{7A9D9CB2-5A72-4610-AB48-E51B9D320089}" name="Name" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{E96E90FF-566D-4FFD-82F1-51DBFC5414D9}" name="Short Name"/>
     <tableColumn id="3" xr3:uid="{40088974-32A7-4DF8-B510-4933C37FC25F}" name="Description"/>
@@ -1876,6 +1882,8 @@
     <tableColumn id="8" xr3:uid="{7294E0AB-9D4B-419B-8BC4-7E9FC9F8EB6C}" name="Trait categories (comma separated)"/>
     <tableColumn id="9" xr3:uid="{7DFF2F95-79C1-4661-9F60-9E1423243B41}" name="Min (only for numeric traits)"/>
     <tableColumn id="10" xr3:uid="{BD24E99B-D835-403D-80DF-6316DD4AD770}" name="Max (only for numeric traits)"/>
+    <tableColumn id="11" xr3:uid="{6E425DC6-2874-4E54-AF1F-1087CC1C7B78}" name="Set size"/>
+    <tableColumn id="12" xr3:uid="{2DF60537-5896-4261-ABCB-3E22583498D5}" name="Is timeseries"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2485,10 +2493,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2505,7 +2513,7 @@
     <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2536,8 +2544,14 @@
       <c r="J1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>457</v>
+      </c>
+      <c r="L1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>116</v>
       </c>
@@ -2556,8 +2570,14 @@
       <c r="G2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>117</v>
       </c>
@@ -2576,8 +2596,14 @@
       <c r="G3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>118</v>
       </c>
@@ -2596,8 +2622,14 @@
       <c r="G4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>119</v>
       </c>
@@ -2616,8 +2648,14 @@
       <c r="G5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>385</v>
       </c>
@@ -2630,8 +2668,14 @@
       <c r="H6" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>386</v>
       </c>
@@ -2643,6 +2687,12 @@
       </c>
       <c r="H7" t="s">
         <v>456</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>